<commit_message>
excel with sample ratios
</commit_message>
<xml_diff>
--- a/Ratios.xlsx
+++ b/Ratios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Estandar\Documents\2. UTDT\29. Datos no estructurados\Clase 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian Estandar\Documents\0. Python\10. Projects\Yahoo Finance Scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06557D2B-BDB3-48A3-8AEB-BBBB3A6E517A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DA5399-49F2-4652-A339-380977F3776D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31785" yWindow="1860" windowWidth="18720" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>AAPL</t>
   </si>
@@ -508,7 +508,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>1.18</v>
+        <v>1.23</v>
       </c>
       <c r="C2" s="6">
         <v>3.28</v>
@@ -571,13 +571,13 @@
         <v>13.19</v>
       </c>
       <c r="E2" s="6">
-        <v>1876000000000</v>
+        <v>2164000000000</v>
       </c>
       <c r="F2" s="6">
-        <v>33.270000000000003</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="G2" s="6">
-        <v>415.9</v>
+        <v>430.06</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -600,19 +600,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="6">
-        <v>2.13</v>
+        <v>2.29</v>
       </c>
       <c r="C3" s="6">
-        <v>74.09</v>
+        <v>76.150000000000006</v>
       </c>
       <c r="D3" s="6">
         <v>0.51</v>
       </c>
       <c r="E3" s="6">
-        <v>99842000000</v>
+        <v>100993000000</v>
       </c>
       <c r="F3" s="6">
-        <v>165.45</v>
+        <v>167.35</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -636,19 +636,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>1.56</v>
+        <v>1.6</v>
       </c>
       <c r="C4" s="6">
-        <v>284.68</v>
+        <v>301.35000000000002</v>
       </c>
       <c r="D4" s="6">
         <v>3.5</v>
       </c>
       <c r="E4" s="6">
-        <v>696983000000</v>
+        <v>767145000000</v>
       </c>
       <c r="F4" s="6">
-        <v>74.98</v>
+        <v>83.49</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -671,8 +671,8 @@
       <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
+      <c r="B5" s="6">
+        <v>1.29</v>
       </c>
       <c r="C5" s="6">
         <v>0.04</v>
@@ -681,10 +681,10 @@
         <v>0.7</v>
       </c>
       <c r="E5" s="6">
-        <v>36088000000</v>
+        <v>30903000000</v>
       </c>
       <c r="F5" s="6">
-        <v>5.79</v>
+        <v>5.24</v>
       </c>
       <c r="G5" s="6">
         <v>6.38</v>
@@ -710,7 +710,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="6">
-        <v>1.3</v>
+        <v>1.26</v>
       </c>
       <c r="C6" s="6">
         <v>5.16</v>
@@ -719,13 +719,13 @@
         <v>-4.66</v>
       </c>
       <c r="E6" s="6">
-        <v>161475000000</v>
+        <v>158309000000</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="6">
-        <v>100.14</v>
+        <v>100.27</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -748,19 +748,19 @@
         <v>16</v>
       </c>
       <c r="B7" s="6">
-        <v>1.2</v>
+        <v>1.21</v>
       </c>
       <c r="C7" s="6">
-        <v>276.95999999999998</v>
+        <v>284.24</v>
       </c>
       <c r="D7" s="6">
         <v>8.18</v>
       </c>
       <c r="E7" s="6">
-        <v>711721000000</v>
+        <v>865785000000</v>
       </c>
       <c r="F7" s="6">
-        <v>30.55</v>
+        <v>37.159999999999997</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -784,16 +784,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>1.87</v>
+        <v>2.06</v>
       </c>
       <c r="C8" s="6">
-        <v>12.67</v>
+        <v>12.11</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="6">
-        <v>2896000000</v>
+        <v>2558000000</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
@@ -820,19 +820,19 @@
         <v>24</v>
       </c>
       <c r="B9" s="6">
-        <v>1.37</v>
+        <v>1.39</v>
       </c>
       <c r="C9" s="6">
-        <v>157</v>
+        <v>166.67</v>
       </c>
       <c r="D9" s="6">
-        <v>1.46</v>
+        <v>1.35</v>
       </c>
       <c r="E9" s="6">
-        <v>7154000000</v>
+        <v>7078000000</v>
       </c>
       <c r="F9" s="6">
-        <v>123.95</v>
+        <v>132.63</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -856,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="6">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C10" s="6">
         <v>3.6</v>
@@ -865,13 +865,13 @@
         <v>7.47</v>
       </c>
       <c r="E10" s="6">
-        <v>291198000000</v>
+        <v>301987000000</v>
       </c>
       <c r="F10" s="6">
-        <v>12.79</v>
+        <v>13.27</v>
       </c>
       <c r="G10" s="6">
-        <v>115.28</v>
+        <v>115.04</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -894,16 +894,16 @@
         <v>20</v>
       </c>
       <c r="B11" s="6">
-        <v>1.69</v>
+        <v>1.71</v>
       </c>
       <c r="C11" s="6">
-        <v>886.62</v>
+        <v>1170.95</v>
       </c>
       <c r="D11" s="6">
-        <v>-4.21</v>
+        <v>-3.4</v>
       </c>
       <c r="E11" s="6">
-        <v>58356000000</v>
+        <v>60444000000</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>10</v>
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="6">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="C12" s="6">
         <v>2.04</v>
@@ -939,10 +939,10 @@
         <v>5.76</v>
       </c>
       <c r="E12" s="6">
-        <v>1614000000000</v>
+        <v>1674000000000</v>
       </c>
       <c r="F12" s="6">
-        <v>37.03</v>
+        <v>38.39</v>
       </c>
       <c r="G12" s="6">
         <v>226.93</v>
@@ -968,19 +968,19 @@
         <v>21</v>
       </c>
       <c r="B13" s="6">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="C13" s="6">
-        <v>509.19</v>
+        <v>515.36</v>
       </c>
       <c r="D13" s="6">
         <v>5.92</v>
       </c>
       <c r="E13" s="6">
-        <v>224759000000</v>
+        <v>241469000000</v>
       </c>
       <c r="F13" s="6">
-        <v>86.06</v>
+        <v>92.46</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1007,13 +1007,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="6">
-        <v>6.56</v>
+        <v>13.02</v>
       </c>
       <c r="D14" s="6">
         <v>-44.1</v>
       </c>
       <c r="E14" s="6">
-        <v>16156000000</v>
+        <v>2421000000</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
@@ -1040,7 +1040,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="6">
-        <v>0.81</v>
+        <v>0.78</v>
       </c>
       <c r="C15" s="6">
         <v>0.98</v>
@@ -1049,13 +1049,13 @@
         <v>1.6</v>
       </c>
       <c r="E15" s="6">
-        <v>151824000000</v>
+        <v>173975000000</v>
       </c>
       <c r="F15" s="6">
-        <v>60.83</v>
+        <v>69.709999999999994</v>
       </c>
       <c r="G15" s="6">
-        <v>110.73</v>
+        <v>112.79</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1078,22 +1078,22 @@
         <v>22</v>
       </c>
       <c r="B16" s="6">
-        <v>1.34</v>
+        <v>1.35</v>
       </c>
       <c r="C16" s="6">
         <v>0.64</v>
       </c>
       <c r="D16" s="6">
-        <v>5.35</v>
+        <v>5.44</v>
       </c>
       <c r="E16" s="6">
-        <v>276203000000</v>
+        <v>315238000000</v>
       </c>
       <c r="F16" s="6">
-        <v>83.96</v>
+        <v>93.85</v>
       </c>
       <c r="G16" s="6">
-        <v>406.18</v>
+        <v>520.92999999999995</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1116,16 +1116,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="6">
-        <v>1.1299999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="C17" s="6">
-        <v>15.54</v>
+        <v>14.76</v>
       </c>
       <c r="D17" s="6">
         <v>397.9</v>
       </c>
       <c r="E17" s="6">
-        <v>1187000000</v>
+        <v>1241000000</v>
       </c>
       <c r="F17" s="6">
         <v>0.03</v>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="6">
-        <v>2.02</v>
+        <v>1.92</v>
       </c>
       <c r="C18" s="6">
         <v>0.35</v>
@@ -1161,13 +1161,13 @@
         <v>10</v>
       </c>
       <c r="E18" s="6">
-        <v>54916000000</v>
+        <v>51537000000</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="6">
-        <v>14.42</v>
+        <v>13.75</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1190,7 +1190,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="6">
-        <v>0.68</v>
+        <v>0.73</v>
       </c>
       <c r="C19" s="6">
         <v>1.52</v>
@@ -1199,13 +1199,13 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="E19" s="6">
-        <v>21325000000</v>
+        <v>211439000000</v>
       </c>
       <c r="F19" s="6">
-        <v>15.2</v>
+        <v>15.06</v>
       </c>
       <c r="G19" s="6">
-        <v>41.85</v>
+        <v>41.79</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1228,16 +1228,16 @@
         <v>8</v>
       </c>
       <c r="B20" s="6">
-        <v>1.8</v>
+        <v>1.89</v>
       </c>
       <c r="C20" s="6">
-        <v>139.36000000000001</v>
+        <v>163.9</v>
       </c>
       <c r="D20" s="6">
-        <v>-0.89</v>
+        <v>-1.1599999999999999</v>
       </c>
       <c r="E20" s="6">
-        <v>20092000000</v>
+        <v>20487000000</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>10</v>
@@ -1264,16 +1264,16 @@
         <v>27</v>
       </c>
       <c r="B21" s="6">
-        <v>1.61</v>
+        <v>1.58</v>
       </c>
       <c r="C21" s="6">
-        <v>1057.05</v>
+        <v>1094.83</v>
       </c>
       <c r="D21" s="6">
         <v>-0.57999999999999996</v>
       </c>
       <c r="E21" s="6">
-        <v>122328000000</v>
+        <v>130336000000</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>10</v>
@@ -1300,19 +1300,19 @@
         <v>3</v>
       </c>
       <c r="B22" s="6">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="C22" s="6">
-        <v>1239.1099999999999</v>
+        <v>1340.18</v>
       </c>
       <c r="D22" s="6">
         <v>1.93</v>
       </c>
       <c r="E22" s="6">
-        <v>27712000000</v>
+        <v>401269000000</v>
       </c>
       <c r="F22" s="6">
-        <v>769.67</v>
+        <v>1114.48</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1336,7 +1336,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="6">
-        <v>1.34</v>
+        <v>1.3</v>
       </c>
       <c r="C23" s="6">
         <v>3.48</v>
@@ -1345,13 +1345,13 @@
         <v>1.68</v>
       </c>
       <c r="E23" s="6">
-        <v>183897000000</v>
+        <v>169171000000</v>
       </c>
       <c r="F23" s="6">
-        <v>25.89</v>
+        <v>23.83</v>
       </c>
       <c r="G23" s="6">
-        <v>47.73</v>
+        <v>48</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1374,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="6">
-        <v>1.71</v>
+        <v>1.75</v>
       </c>
       <c r="C24" s="6">
         <v>0.14000000000000001</v>
@@ -1383,13 +1383,13 @@
         <v>3.12</v>
       </c>
       <c r="E24" s="6">
-        <v>2863000000</v>
+        <v>2187000000</v>
       </c>
       <c r="F24" s="6">
-        <v>2.1800000000000002</v>
+        <v>1.78</v>
       </c>
       <c r="G24" s="6">
-        <v>7.96</v>
+        <v>7.13</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>

</xml_diff>